<commit_message>
Update till Track Order
</commit_message>
<xml_diff>
--- a/TestData/OrderTestData/orderTestCase.xlsx
+++ b/TestData/OrderTestData/orderTestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\OrderTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CA5F35-B64F-449A-8F60-4630F60529A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE445DC7-986D-44A6-9F11-C02071248EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,36 +385,6 @@
     <t>abced Test 5</t>
   </si>
   <si>
-    <t>9881012051</t>
-  </si>
-  <si>
-    <t>9881012052</t>
-  </si>
-  <si>
-    <t>9881012053</t>
-  </si>
-  <si>
-    <t>9881012054</t>
-  </si>
-  <si>
-    <t>9881012055</t>
-  </si>
-  <si>
-    <t>testuser151@mail.com</t>
-  </si>
-  <si>
-    <t>testuser152@mail.com</t>
-  </si>
-  <si>
-    <t>testuser153@mail.com</t>
-  </si>
-  <si>
-    <t>testuser154@mail.com</t>
-  </si>
-  <si>
-    <t>testuser155@mail.com</t>
-  </si>
-  <si>
     <t>searchValue</t>
   </si>
   <si>
@@ -431,6 +401,36 @@
   </si>
   <si>
     <t>223</t>
+  </si>
+  <si>
+    <t>9881012056</t>
+  </si>
+  <si>
+    <t>9881012057</t>
+  </si>
+  <si>
+    <t>9881012058</t>
+  </si>
+  <si>
+    <t>9881012059</t>
+  </si>
+  <si>
+    <t>9881012060</t>
+  </si>
+  <si>
+    <t>testuser156@mail.com</t>
+  </si>
+  <si>
+    <t>testuser157@mail.com</t>
+  </si>
+  <si>
+    <t>testuser158@mail.com</t>
+  </si>
+  <si>
+    <t>testuser159@mail.com</t>
+  </si>
+  <si>
+    <t>testuser160@mail.com</t>
   </si>
 </sst>
 </file>
@@ -2392,13 +2392,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>111</v>
@@ -2481,13 +2481,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>112</v>
@@ -2570,13 +2570,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>111</v>
@@ -2659,13 +2659,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>112</v>
@@ -2748,13 +2748,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>112</v>
@@ -2852,7 +2852,7 @@
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="X2" sqref="A1:Y6"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3348,7 +3348,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -3374,7 +3374,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
@@ -3400,7 +3400,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>34</v>
@@ -3426,7 +3426,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>35</v>
@@ -3452,7 +3452,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>36</v>
@@ -3478,7 +3478,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Inventory Section with 60% Done
</commit_message>
<xml_diff>
--- a/TestData/OrderTestData/orderTestCase.xlsx
+++ b/TestData/OrderTestData/orderTestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\OrderTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE445DC7-986D-44A6-9F11-C02071248EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D67C728-9668-4BF7-BE89-2EA4D34B31BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,34 +403,34 @@
     <t>223</t>
   </si>
   <si>
-    <t>9881012056</t>
-  </si>
-  <si>
-    <t>9881012057</t>
-  </si>
-  <si>
-    <t>9881012058</t>
-  </si>
-  <si>
-    <t>9881012059</t>
-  </si>
-  <si>
-    <t>9881012060</t>
-  </si>
-  <si>
-    <t>testuser156@mail.com</t>
-  </si>
-  <si>
-    <t>testuser157@mail.com</t>
-  </si>
-  <si>
-    <t>testuser158@mail.com</t>
-  </si>
-  <si>
-    <t>testuser159@mail.com</t>
-  </si>
-  <si>
-    <t>testuser160@mail.com</t>
+    <t>9881012066</t>
+  </si>
+  <si>
+    <t>9881012067</t>
+  </si>
+  <si>
+    <t>9881012068</t>
+  </si>
+  <si>
+    <t>9881012069</t>
+  </si>
+  <si>
+    <t>9881012070</t>
+  </si>
+  <si>
+    <t>testuser166@mail.com</t>
+  </si>
+  <si>
+    <t>testuser167@mail.com</t>
+  </si>
+  <si>
+    <t>testuser168@mail.com</t>
+  </si>
+  <si>
+    <t>testuser169@mail.com</t>
+  </si>
+  <si>
+    <t>testuser170@mail.com</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1293,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2:X6"/>
     </sheetView>
   </sheetViews>
@@ -1796,7 +1796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECFF00E-9730-4B45-8873-16E5E2653898}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -2259,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75904CA-780D-4078-9ECB-A0AE5CFCF05B}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2851,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C688C3D-51E4-4D9C-BBCF-CA6AF3FBDF3A}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X2:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>